<commit_message>
student page done minus request equipment
</commit_message>
<xml_diff>
--- a/src/main/resources/Book 2.xlsx
+++ b/src/main/resources/Book 2.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{319A792A-32B6-4CEE-8E80-8C6A930BAB6A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BC3850A-B622-4460-97CD-31556E7D8CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>id</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>test2</t>
   </si>
 </sst>
 </file>
@@ -403,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -457,6 +460,29 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>